<commit_message>
DG38-287 | feat: updates heuristics implementation to take into account all staff; updates complexity-analysis file.
</commit_message>
<xml_diff>
--- a/Planning/analysis/complexity-analysis.xlsx
+++ b/Planning/analysis/complexity-analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\IdeaProjects\3ANO_1SEMESTRE\sem5pi-2425-dg38\Planning\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{838323D6-CDE8-4EF4-9E94-23C73DE1DEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B7DF62-92AD-4142-8607-A7CF07A6A220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{FC77DE42-337C-436A-9083-507E690903F2}"/>
   </bookViews>
   <sheets>
     <sheet name="With doctors+TSurgeryOnly" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>N. of Surgeries</t>
   </si>
@@ -95,9 +96,6 @@
     <t>Time to generate the heuristic solution(s)</t>
   </si>
   <si>
-    <t>Solution with the Heuristic</t>
-  </si>
-  <si>
     <t>Final Time for the last Surgery Using Heuristic (minutes)</t>
   </si>
   <si>
@@ -144,13 +142,94 @@
   </si>
   <si>
     <t>RESULTS FOR ALGORITHMS WITH ONLY DOCTORS AND TSURGERY</t>
+  </si>
+  <si>
+    <t>Solution with the Heuristic (Criteria 1)</t>
+  </si>
+  <si>
+    <t>Solution with the Heuristic (Criteria 2)</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(595,669,so100005),(750,780,mnt0001),(791,850,so100001),(851,910,so100006),(961,1050,so100002),(1080,1110,mnt0002),(1141,1200,so100004)]</t>
+  </si>
+  <si>
+    <t>0.0020</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(595,669,so100005),(750,780,mnt0001),(791,880,so100007),(881,940,so100001),(961,1050,so100002),(1080,1110,mnt0002),(1141,1200,so100004)]</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(595,684,so100002),(750,780,mnt0001),(791,850,so100001),(1080,1110,mnt0002)]</t>
+  </si>
+  <si>
+    <t>0.00083</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(595,684,so100002),(750,780,mnt0001),(791,850,so100001),(961,1020,so100004),(1080,1110,mnt0002)]</t>
+  </si>
+  <si>
+    <t>0.0017</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(595,669,so100005),(750,780,mnt0001),(791,850,so100001),(961,1050,so100002),(1080,1110,mnt0002),(1141,1200,so100004)]</t>
+  </si>
+  <si>
+    <t>0.0018</t>
+  </si>
+  <si>
+    <t>couldnt schedule 6</t>
+  </si>
+  <si>
+    <t>0.0023</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(620,679,so100008),(750,780,mnt0001),(791,880,so100007),(881,940,so100001),(981,1055,so100005),(1080,1110,mnt0002),(1111,1200,so100002)]</t>
+  </si>
+  <si>
+    <t>0.0027</t>
+  </si>
+  <si>
+    <t>couldnt schedule 6 &amp; 8</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(620,679,so100008),(680,739,so100009),(750,780,mnt0001),(791,880,so100007),(881,940,so100001),(981,1055,so100005),(1080,1110,mnt0002),(1111,1200,so100002)]</t>
+  </si>
+  <si>
+    <t>couldnt schedule 6 &amp; 4</t>
+  </si>
+  <si>
+    <t>0.0029</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(620,679,so100008),(680,739,so100009),(750,780,mnt0001),(791,880,so100007),(881,940,so100001),(981,1055,so100005),(1080,1110,mnt0002),(1111,1170,so100010),(1171,1260,so100002)]</t>
+  </si>
+  <si>
+    <t>0.0036</t>
+  </si>
+  <si>
+    <t>0.0032</t>
+  </si>
+  <si>
+    <t>couldnt schedule 6 &amp; 4 &amp; 11</t>
+  </si>
+  <si>
+    <t>0.0042</t>
+  </si>
+  <si>
+    <t>couldnt schedule 6 &amp; 4 &amp; 11 &amp; 12</t>
+  </si>
+  <si>
+    <t>[(520,594,so100003),(620,679,so100008),(680,739,so100009),(750,780,mnt0001),(781,840,so100013),(841,900,so100010),(901,960,so100001),(981,1055,so100005),(1080,1110,mnt0002),(1111,1200,so100007),(1201,1290,so100002)]</t>
+  </si>
+  <si>
+    <t>0.0040</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +257,12 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -402,9 +487,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -413,22 +496,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -438,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -504,21 +572,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -855,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8BCB14-614B-4528-8997-57B4C37B4EA1}">
-  <dimension ref="A2:I19"/>
+  <dimension ref="A2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="J31" sqref="B5:J31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="54" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -871,54 +935,56 @@
     <col min="7" max="7" width="61.9296875" customWidth="1"/>
     <col min="8" max="8" width="30.3984375" customWidth="1"/>
     <col min="9" max="9" width="24.1328125" customWidth="1"/>
+    <col min="10" max="10" width="63.265625" customWidth="1"/>
+    <col min="11" max="11" width="36.796875" customWidth="1"/>
+    <col min="12" max="12" width="21.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="23"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="23"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B6" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
+    <row r="6" spans="1:13" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="B6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:9" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
@@ -932,19 +998,28 @@
         <v>3</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>19</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>20</v>
       </c>
       <c r="I7" s="22" t="s">
         <v>18</v>
       </c>
+      <c r="J7" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B8" s="6">
         <v>3</v>
       </c>
@@ -966,10 +1041,19 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="2">
+        <v>850</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B9" s="6">
         <f t="shared" ref="B9:B18" si="0">B8+1</f>
         <v>4</v>
@@ -988,16 +1072,25 @@
         <v>7</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="2">
         <v>1020</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="2">
+        <v>850</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1016,16 +1109,25 @@
         <v>9</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2">
         <v>1185</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="2">
+        <v>850</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B11" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1044,16 +1146,25 @@
         <v>11</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="2">
         <v>1185</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="2">
+        <v>910</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B12" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1072,16 +1183,28 @@
         <v>12</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="2">
         <v>1275</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="2">
+        <v>940</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1102,10 +1225,22 @@
       <c r="G13" s="19"/>
       <c r="H13" s="2"/>
       <c r="I13" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="2">
+        <v>940</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1115,19 +1250,31 @@
         <v>362880</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="2">
         <v>1260</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="2"/>
       <c r="I14" s="18"/>
+      <c r="J14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="2">
+        <v>940</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1142,8 +1289,20 @@
       <c r="G15" s="19"/>
       <c r="H15" s="2"/>
       <c r="I15" s="18"/>
+      <c r="J15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="2">
+        <v>940</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1158,8 +1317,20 @@
       <c r="G16" s="19"/>
       <c r="H16" s="2"/>
       <c r="I16" s="18"/>
+      <c r="J16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="2">
+        <v>940</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1174,8 +1345,20 @@
       <c r="G17" s="19"/>
       <c r="H17" s="2"/>
       <c r="I17" s="18"/>
+      <c r="J17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="2">
+        <v>940</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="18" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:13" ht="57.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B18" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1190,14 +1373,39 @@
       <c r="G18" s="20"/>
       <c r="H18" s="10"/>
       <c r="I18" s="21"/>
+      <c r="J18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="10">
+        <v>960</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="19" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="2:13" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B6:L6"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E93C697-6550-4DA9-B9B1-CA444444B90F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1435,20 +1643,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b163ee49-d5ca-4566-8d9a-132778b8595f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b163ee49-d5ca-4566-8d9a-132778b8595f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1471,14 +1679,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E39BA9-671A-4545-8A5C-A950D637590C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4574B1A7-38A6-4D05-AD02-7C2F28771731}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b163ee49-d5ca-4566-8d9a-132778b8595f"/>
@@ -1493,4 +1693,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E39BA9-671A-4545-8A5C-A950D637590C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>